<commit_message>
Clustertest experiment, and final release 2.2 of ctmixtures, for all of the experiments.  Timing analysis to understand costs of the experiments
</commit_message>
<xml_diff>
--- a/explorations/timing-analysis.xlsx
+++ b/explorations/timing-analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31540" windowHeight="20800" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="5180" yWindow="940" windowWidth="31540" windowHeight="20800" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original calcs" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Min to run</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>C3.2xlarge</t>
+  </si>
+  <si>
+    <t>EC2 c3.xlarge execution 260 sec</t>
+  </si>
+  <si>
+    <t>c3.xlarge</t>
+  </si>
+  <si>
+    <t>StarCluster execution test (real data)</t>
+  </si>
+  <si>
+    <t>Data from MBP laptop testing</t>
   </si>
 </sst>
 </file>
@@ -248,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -286,8 +298,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -313,8 +455,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3"/>
@@ -331,8 +487,30 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="9" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="10" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="11" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="12" xfId="24" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="39">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
     <cellStyle name="Currency" xfId="24" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -345,6 +523,13 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
@@ -355,6 +540,13 @@
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -1303,288 +1495,325 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E33"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
-    <col min="2" max="5" width="33" customWidth="1"/>
+    <col min="2" max="3" width="33" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5">
-      <c r="B4" t="s">
+    <row r="2" spans="1:7">
+      <c r="B2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="5" spans="1:7">
+      <c r="B5" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="26">
         <v>200000</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="27">
+        <v>100000</v>
+      </c>
+      <c r="F7" s="1">
         <v>200000</v>
       </c>
-      <c r="D7" s="1">
-        <v>300000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G7" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="26">
+        <v>4.3</v>
+      </c>
+      <c r="C8" s="27">
+        <v>4.3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="E9" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="B9" s="26">
+        <v>10</v>
+      </c>
+      <c r="C9" s="27">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1">
+        <v>10</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="28">
+        <f>B9*B21</f>
+        <v>40</v>
+      </c>
+      <c r="C10" s="29">
+        <f>C9*C21</f>
+        <v>40</v>
+      </c>
+      <c r="F10" s="2">
+        <f>F9*F21</f>
+        <v>40</v>
+      </c>
+      <c r="G10" s="2">
+        <f>G9*G21</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="1">
-        <v>6</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1">
+        <v>36</v>
+      </c>
+      <c r="B11" s="28">
+        <f>60/B8</f>
+        <v>13.953488372093023</v>
+      </c>
+      <c r="C11" s="29">
+        <f>60/C8</f>
+        <v>13.953488372093023</v>
+      </c>
+      <c r="F11" s="2">
+        <f>60/F8</f>
+        <v>24</v>
+      </c>
+      <c r="G11" s="2">
+        <f>60/G8</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="28">
+        <f>B11 * B21</f>
+        <v>55.813953488372093</v>
+      </c>
+      <c r="C12" s="29">
+        <f>C11 * C21</f>
+        <v>55.813953488372093</v>
+      </c>
+      <c r="F12" s="2">
+        <f>F11 * F21</f>
+        <v>96</v>
+      </c>
+      <c r="G12" s="2">
+        <f>G11 * G21</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="28">
+        <f>B7 / (B12*B9)</f>
+        <v>358.33333333333337</v>
+      </c>
+      <c r="C13" s="29">
+        <f>C7 / (C12*C9)</f>
+        <v>179.16666666666669</v>
+      </c>
+      <c r="F13" s="2">
+        <f>F7 / (F12*F9)</f>
+        <v>208.33333333333334</v>
+      </c>
+      <c r="G13" s="2">
+        <f>G7 / (G12*G9)</f>
+        <v>173.61111111111111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="30">
+        <f>B13/24</f>
+        <v>14.930555555555557</v>
+      </c>
+      <c r="C14" s="31">
+        <f>C13/24</f>
+        <v>7.4652777777777786</v>
+      </c>
+      <c r="F14" s="11">
+        <f>F13/24</f>
+        <v>8.6805555555555554</v>
+      </c>
+      <c r="G14" s="11">
+        <f>G13/24</f>
+        <v>7.2337962962962967</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="28">
+        <f>B13*B9</f>
+        <v>3583.3333333333339</v>
+      </c>
+      <c r="C15" s="29">
+        <f>C13*C9</f>
+        <v>1791.666666666667</v>
+      </c>
+      <c r="F15" s="2">
+        <f>F13*F9</f>
+        <v>2083.3333333333335</v>
+      </c>
+      <c r="G15" s="2">
+        <f>G13*G9</f>
+        <v>1041.6666666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="20">
+        <f>B15*B22</f>
+        <v>752.50000000000011</v>
+      </c>
+      <c r="C16" s="21">
+        <f>C15*C22</f>
+        <v>376.25000000000006</v>
+      </c>
+      <c r="F16" s="13">
+        <f>F15*F22</f>
+        <v>437.5</v>
+      </c>
+      <c r="G16" s="13">
+        <f>G15*G22</f>
+        <v>437.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="18">
+        <v>4</v>
+      </c>
+      <c r="C21" s="19">
+        <v>4</v>
+      </c>
+      <c r="F21" s="1">
+        <v>4</v>
+      </c>
+      <c r="G21" s="1">
         <v>8</v>
       </c>
-      <c r="E11" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="2">
-        <f>B11*B32</f>
-        <v>24</v>
-      </c>
-      <c r="C13" s="2">
-        <f>C11*C32</f>
-        <v>48</v>
-      </c>
-      <c r="D13" s="2">
-        <f>D11*D32</f>
-        <v>64</v>
-      </c>
-      <c r="E13" s="2">
-        <f>E11*E32</f>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="2">
-        <f>60/B9</f>
-        <v>24</v>
-      </c>
-      <c r="C15" s="2">
-        <f>60/C9</f>
-        <v>24</v>
-      </c>
-      <c r="D15" s="2">
-        <f>60/D9</f>
-        <v>24</v>
-      </c>
-      <c r="E15" s="2">
-        <f>60/E9</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" s="2">
-        <f>B15 * B32</f>
-        <v>96</v>
-      </c>
-      <c r="C17" s="2">
-        <f>C15 * C32</f>
-        <v>192</v>
-      </c>
-      <c r="D17" s="2">
-        <f>D15 * D32</f>
-        <v>192</v>
-      </c>
-      <c r="E17" s="2">
-        <f>E15 * E32</f>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="2">
-        <f>B7 / (B17*B11)</f>
-        <v>347.22222222222223</v>
-      </c>
-      <c r="C19" s="2">
-        <f>C7 / (C17*C11)</f>
-        <v>173.61111111111111</v>
-      </c>
-      <c r="D19" s="2">
-        <f>D7 / (D17*D11)</f>
-        <v>195.3125</v>
-      </c>
-      <c r="E19" s="2">
-        <f>E7 / (E17*E11)</f>
-        <v>325.52083333333331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="11">
-        <f>B19/24</f>
-        <v>14.467592592592593</v>
-      </c>
-      <c r="C21" s="11">
-        <f>C19/24</f>
-        <v>7.2337962962962967</v>
-      </c>
-      <c r="D21" s="11">
-        <f>D19/24</f>
-        <v>8.1380208333333339</v>
-      </c>
-      <c r="E21" s="11">
-        <f>E19/24</f>
-        <v>13.563368055555555</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="2">
-        <f>B19*B11</f>
-        <v>2083.3333333333335</v>
-      </c>
-      <c r="C23" s="2">
-        <f>C19*C11</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="D23" s="2">
-        <f>D19*D11</f>
-        <v>1562.5</v>
-      </c>
-      <c r="E23" s="2">
-        <f>E19*E11</f>
-        <v>2604.1666666666665</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="13">
-        <f>B23*B33</f>
-        <v>437.5</v>
-      </c>
-      <c r="C25" s="13">
-        <f>C23*C33</f>
-        <v>437.5</v>
-      </c>
-      <c r="D25" s="13">
-        <f>D23*D33</f>
-        <v>656.25</v>
-      </c>
-      <c r="E25" s="13">
-        <f>E23*E33</f>
-        <v>1093.75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="1">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1">
-        <v>8</v>
-      </c>
-      <c r="D32" s="1">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B22" s="24">
         <v>0.21</v>
       </c>
-      <c r="C33" s="12">
-        <v>0.42</v>
-      </c>
-      <c r="D33" s="12">
-        <v>0.42</v>
-      </c>
-      <c r="E33" s="12">
+      <c r="C22" s="25">
+        <v>0.21</v>
+      </c>
+      <c r="F22" s="12">
+        <v>0.21</v>
+      </c>
+      <c r="G22" s="12">
         <v>0.42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Full configuration for equifinality-1, a 40K batch over 4 models (3 mixtures and 1 neutral).  Uses ctmixtures-2.3.
</commit_message>
<xml_diff>
--- a/explorations/timing-analysis.xlsx
+++ b/explorations/timing-analysis.xlsx
@@ -1498,7 +1498,7 @@
   <dimension ref="A2:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1555,7 +1555,7 @@
         <v>200000</v>
       </c>
       <c r="C7" s="27">
-        <v>100000</v>
+        <v>40000</v>
       </c>
       <c r="F7" s="1">
         <v>200000</v>
@@ -1589,7 +1589,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9" s="1">
         <v>10</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="C10" s="29">
         <f>C9*C21</f>
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2">
         <f>F9*F21</f>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="C13" s="29">
         <f>C7 / (C12*C9)</f>
-        <v>179.16666666666669</v>
+        <v>89.583333333333329</v>
       </c>
       <c r="F13" s="2">
         <f>F7 / (F12*F9)</f>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C14" s="31">
         <f>C13/24</f>
-        <v>7.4652777777777786</v>
+        <v>3.7326388888888888</v>
       </c>
       <c r="F14" s="11">
         <f>F13/24</f>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C15" s="29">
         <f>C13*C9</f>
-        <v>1791.666666666667</v>
+        <v>716.66666666666663</v>
       </c>
       <c r="F15" s="2">
         <f>F13*F9</f>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C16" s="21">
         <f>C15*C22</f>
-        <v>376.25000000000006</v>
+        <v>150.5</v>
       </c>
       <c r="F16" s="13">
         <f>F15*F22</f>

</xml_diff>

<commit_message>
verification of Moran mutation rates and testing, for ctmixtures 2.4.  equifinality-2 will use ctmixtures 2.4 and pytransmission 1.0 and redo equifinality-1 but with the corrected Moran mutation rates
</commit_message>
<xml_diff>
--- a/explorations/timing-analysis.xlsx
+++ b/explorations/timing-analysis.xlsx
@@ -1497,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1572,7 +1572,7 @@
         <v>4.3</v>
       </c>
       <c r="C8" s="27">
-        <v>4.3</v>
+        <v>3</v>
       </c>
       <c r="F8" s="1">
         <v>2.5</v>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="C11" s="29">
         <f>60/C8</f>
-        <v>13.953488372093023</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2">
         <f>60/F8</f>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C12" s="29">
         <f>C11 * C21</f>
-        <v>55.813953488372093</v>
+        <v>80</v>
       </c>
       <c r="F12" s="2">
         <f>F11 * F21</f>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="C13" s="29">
         <f>C7 / (C12*C9)</f>
-        <v>89.583333333333329</v>
+        <v>62.5</v>
       </c>
       <c r="F13" s="2">
         <f>F7 / (F12*F9)</f>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C14" s="31">
         <f>C13/24</f>
-        <v>3.7326388888888888</v>
+        <v>2.6041666666666665</v>
       </c>
       <c r="F14" s="11">
         <f>F13/24</f>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="C15" s="29">
         <f>C13*C9</f>
-        <v>716.66666666666663</v>
+        <v>500</v>
       </c>
       <c r="F15" s="2">
         <f>F13*F9</f>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="C16" s="21">
         <f>C15*C22</f>
-        <v>150.5</v>
+        <v>105</v>
       </c>
       <c r="F16" s="13">
         <f>F15*F22</f>

</xml_diff>

<commit_message>
performed a lot of tests to verify the accuracy of the amount of variation in the neutral models, and I understand what's happening now.  4MM is a good value for quasi-stationarity in the neutral model, and I'll use that for ongoing experiments.
</commit_message>
<xml_diff>
--- a/explorations/timing-analysis.xlsx
+++ b/explorations/timing-analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Min to run</t>
   </si>
@@ -151,13 +151,19 @@
     <t>EC2 c3.xlarge execution 260 sec</t>
   </si>
   <si>
-    <t>c3.xlarge</t>
-  </si>
-  <si>
     <t>StarCluster execution test (real data)</t>
   </si>
   <si>
     <t>Data from MBP laptop testing</t>
+  </si>
+  <si>
+    <t>CTMixtures N=100, KI=50, 4MM steps</t>
+  </si>
+  <si>
+    <t>EC2 c3.4xlarge</t>
+  </si>
+  <si>
+    <t>c3.4xlarge</t>
   </si>
 </sst>
 </file>
@@ -1497,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1510,11 +1516,11 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="B2" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="15"/>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1523,7 +1529,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="B4" s="16" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>35</v>
@@ -1537,7 +1543,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" s="16" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>42</v>
@@ -1552,7 +1558,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="26">
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="C7" s="27">
         <v>40000</v>
@@ -1569,10 +1575,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="26">
-        <v>4.3</v>
+        <v>3.3</v>
       </c>
       <c r="C8" s="27">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="F8" s="1">
         <v>2.5</v>
@@ -1586,10 +1592,10 @@
         <v>27</v>
       </c>
       <c r="B9" s="26">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C9" s="27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1">
         <v>10</v>
@@ -1604,11 +1610,11 @@
       </c>
       <c r="B10" s="28">
         <f>B9*B21</f>
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="C10" s="29">
         <f>C9*C21</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F10" s="2">
         <f>F9*F21</f>
@@ -1625,11 +1631,11 @@
       </c>
       <c r="B11" s="28">
         <f>60/B8</f>
-        <v>13.953488372093023</v>
+        <v>18.181818181818183</v>
       </c>
       <c r="C11" s="29">
         <f>60/C8</f>
-        <v>20</v>
+        <v>18.181818181818183</v>
       </c>
       <c r="F11" s="2">
         <f>60/F8</f>
@@ -1646,11 +1652,11 @@
       </c>
       <c r="B12" s="28">
         <f>B11 * B21</f>
-        <v>55.813953488372093</v>
+        <v>290.90909090909093</v>
       </c>
       <c r="C12" s="29">
         <f>C11 * C21</f>
-        <v>80</v>
+        <v>290.90909090909093</v>
       </c>
       <c r="F12" s="2">
         <f>F11 * F21</f>
@@ -1667,11 +1673,11 @@
       </c>
       <c r="B13" s="28">
         <f>B7 / (B12*B9)</f>
-        <v>358.33333333333337</v>
+        <v>85.937499999999986</v>
       </c>
       <c r="C13" s="29">
         <f>C7 / (C12*C9)</f>
-        <v>62.5</v>
+        <v>34.375</v>
       </c>
       <c r="F13" s="2">
         <f>F7 / (F12*F9)</f>
@@ -1688,11 +1694,11 @@
       </c>
       <c r="B14" s="30">
         <f>B13/24</f>
-        <v>14.930555555555557</v>
+        <v>3.5807291666666661</v>
       </c>
       <c r="C14" s="31">
         <f>C13/24</f>
-        <v>2.6041666666666665</v>
+        <v>1.4322916666666667</v>
       </c>
       <c r="F14" s="11">
         <f>F13/24</f>
@@ -1709,11 +1715,11 @@
       </c>
       <c r="B15" s="28">
         <f>B13*B9</f>
-        <v>3583.3333333333339</v>
+        <v>343.74999999999994</v>
       </c>
       <c r="C15" s="29">
         <f>C13*C9</f>
-        <v>500</v>
+        <v>137.5</v>
       </c>
       <c r="F15" s="2">
         <f>F13*F9</f>
@@ -1730,11 +1736,11 @@
       </c>
       <c r="B16" s="20">
         <f>B15*B22</f>
-        <v>752.50000000000011</v>
+        <v>288.74999999999994</v>
       </c>
       <c r="C16" s="21">
         <f>C15*C22</f>
-        <v>105</v>
+        <v>115.5</v>
       </c>
       <c r="F16" s="13">
         <f>F15*F22</f>
@@ -1765,10 +1771,10 @@
         <v>31</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>34</v>
@@ -1782,10 +1788,10 @@
         <v>32</v>
       </c>
       <c r="B21" s="18">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C21" s="19">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
@@ -1799,10 +1805,10 @@
         <v>33</v>
       </c>
       <c r="B22" s="24">
-        <v>0.21</v>
+        <v>0.84</v>
       </c>
       <c r="C22" s="25">
-        <v>0.21</v>
+        <v>0.84</v>
       </c>
       <c r="F22" s="12">
         <v>0.21</v>

</xml_diff>

<commit_message>
Equifinality 3 analysis underway
</commit_message>
<xml_diff>
--- a/explorations/timing-analysis.xlsx
+++ b/explorations/timing-analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Min to run</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>c3.4xlarge</t>
+  </si>
+  <si>
+    <t>Actual instance hours</t>
+  </si>
+  <si>
+    <t>Actual cost for compute</t>
   </si>
 </sst>
 </file>
@@ -1501,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A2:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1817,6 +1823,22 @@
         <v>0.42</v>
       </c>
     </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>344.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>